<commit_message>
Updated w more re: sessions
</commit_message>
<xml_diff>
--- a/scripts/reinvent-schedule.xlsx
+++ b/scripts/reinvent-schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mwvaughn/src/websites/day1hpc.github.io/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC6940E-563F-374D-8CBB-B1BA3CFE6272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BCE8CB-5CBE-C940-8FF0-DA391369CD4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28580" windowHeight="16520" xr2:uid="{D53CFD4F-014A-B641-809F-A5757838F61D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16640" xr2:uid="{D53CFD4F-014A-B641-809F-A5757838F61D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="192">
   <si>
     <t>Title</t>
   </si>
@@ -329,9 +329,6 @@
     <t>Dow</t>
   </si>
   <si>
-    <t>Batch, Containers, Kubernetes</t>
-  </si>
-  <si>
     <t>HPC, Machine Learning</t>
   </si>
   <si>
@@ -341,16 +338,277 @@
     <t>Graviton, Arm, Developer Tools</t>
   </si>
   <si>
-    <t>HPC, ParallelCluster, Batch, EFA</t>
-  </si>
-  <si>
     <t>HPC, CFD, CAE</t>
   </si>
   <si>
     <t>ParallelCluster, EFA, Machine Learning</t>
   </si>
   <si>
-    <t>HPC, ParallelCluster, Batch, Geospatial, Open Data</t>
+    <t>CMP211-R</t>
+  </si>
+  <si>
+    <t>A framework for physics-informed neural networks on PyTorch</t>
+  </si>
+  <si>
+    <t>In this chalk talk, learn about a new physics-informed neural network (PINNs) framework for simulations on PyTorch for fast-to-compute and highly accurate models for various applications. The computational cost associated with multi-physics simulations often impose serious limitations for design space exploration, optimization, and uncertainty quantification. Learn how to apply methods for solving partial differential equations that govern the physics of engineering systems using PINNs and other relevant applications in engineering. This was developed and implemented by AWS in collaboration with the University of Central Florida.</t>
+  </si>
+  <si>
+    <t>Ana Simoes, Principal Specialist, ML Frameworks, Amazon</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Level 1, Forum 104, Caesars Forum</t>
+  </si>
+  <si>
+    <t>Machine Learning, EFA</t>
+  </si>
+  <si>
+    <t>STG343</t>
+  </si>
+  <si>
+    <t>Deep dive on accelerating HPC and ML with Amazon FSx</t>
+  </si>
+  <si>
+    <t>File services are often asked to deliver performant capabilities with low latencies for compute-intensive workloads or high IOPS for data-intensive applications. In this session, learn best practices for choosing how to rightsize your performance, reduce latency, increase throughput, and optimize cost. The Amazon FSx family of managed file storage services provides feature sets and performance profiles supporting a variety of use cases. Many workloads like machine learning (ML), high performance computing (HPC), video rendering, and financial analytics require cost optimizations and deployment options. This session also shares tips and best practices for migrating performant-dependent use cases to AWS.</t>
+  </si>
+  <si>
+    <t>Shrinath Kurdekar, Principal Solutions Architect</t>
+  </si>
+  <si>
+    <t>Level 1 North, South Pacific F, Mandalay Bay</t>
+  </si>
+  <si>
+    <t>Storage, Lustre, HPC, Machine Learning</t>
+  </si>
+  <si>
+    <t>CMP331-R</t>
+  </si>
+  <si>
+    <t>High-throughput computing for financial risk management and modeling</t>
+  </si>
+  <si>
+    <t>In this chalk talk, explore how financial services industry organizations can achieve greater elasticity, higher throughput, and significant cost savings with a cloud-native high-throughput computing (HTC) grid solution built on AWS core services. Using modular architecture made up of managed services such as Amazon EKS, Amazon DynamoDB, Amazon SQS, and Amazon EC2 Spot Instances, HTC grid solutions dynamically scale computing resources to meet the demanding throughput requirements of risk-analytics workloads. Join the talk to learn about the modular architecture, scalability, and performance you can achieve with this solution.</t>
+  </si>
+  <si>
+    <t>Kirill Bogdanov, Sr. Solutions Architect</t>
+  </si>
+  <si>
+    <t>Mark Norton, Principal EC2 &amp; HPC Specialist</t>
+  </si>
+  <si>
+    <t>Level 1, Room 101, MGM Grand</t>
+  </si>
+  <si>
+    <t>FSI, HTC</t>
+  </si>
+  <si>
+    <t>CMP320</t>
+  </si>
+  <si>
+    <t>Accelerating semiconductor design, simulation, and verification</t>
+  </si>
+  <si>
+    <t>AWS offers many solutions to design, simulate, and verify the advanced semiconductor devices that are the foundation of modern technology. Electronic design automation (EDA) workloads are critical to the success of chip development. EDA requires computing for digital and analog simulations, logic synthesis, design rule checks, and physical verification. In this session, discover best practices for running HPC or EDA workloads on AWS using Amazon EC2. Hear from Arm about how they use AWS to accelerate EDA workloads in the cloud using Arm-based AWS Graviton instances. Also, Marvell shares how they’re using EDA in the cloud to scale their highly differentiated cloud-optimized silicon solutions for customers like AWS.</t>
+  </si>
+  <si>
+    <t>Arm</t>
+  </si>
+  <si>
+    <t>William Cornwell, VP of Engineering</t>
+  </si>
+  <si>
+    <t>Marvell</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Level 1, Grand 115, MGM Grand</t>
+  </si>
+  <si>
+    <t>EDA, HPC</t>
+  </si>
+  <si>
+    <t>Level 1, Boulevard 169, MGM Grand</t>
+  </si>
+  <si>
+    <t>ENU402</t>
+  </si>
+  <si>
+    <t>Modernizing HPC workloads using AWS services</t>
+  </si>
+  <si>
+    <t>For decades, industries have been using high-performance computing (HPC) to solve problems that are not solvable on a single machine or to shorten problem-solving run time. Traditionally, HPC workloads are launched and managed on the master node, which represents a single point of failure. Building HPC clusters on AWS allows you to keep the same user experience of launching, monitoring, and managing an HPC workload. In this chalk talk, learn how to launch, monitor, and manage an HPC workload using native AWS services, following a seismic processing problem as an example.</t>
+  </si>
+  <si>
+    <t>Cyril Lagrange, Solution Architect</t>
+  </si>
+  <si>
+    <t>Kun Jiao, Energy Principal Solutions Architect</t>
+  </si>
+  <si>
+    <t>HPC</t>
+  </si>
+  <si>
+    <t>PRT220</t>
+  </si>
+  <si>
+    <t>How to maximize HPC productivity, performance, and portability (sponsored by NVIDIA)</t>
+  </si>
+  <si>
+    <t>In this session, learn how NVIDIA enables high-performance computing (HPC) on over 200 Amazon EC2 instance types. NVIDIA provides a multi-platform, standards-compliant, vendor-supported solution for HPC application development that supports all major programming models. Its proven compilers, libraries, and software tools support AWS Graviton to maximize developer productivity, enable hardware platform choice, and facilitate an optimal price-performance solution for HPC applications in the cloud. This presentation is brought to you by NVIDIA, an AWS Partner.</t>
+  </si>
+  <si>
+    <t>John Linford, Technical Product Manager CPU Software</t>
+  </si>
+  <si>
+    <t>NVIDIA</t>
+  </si>
+  <si>
+    <t>Level 3 South, South Seas C, Mandalay Bay</t>
+  </si>
+  <si>
+    <t>HPC, Arm, Graviton</t>
+  </si>
+  <si>
+    <t>ENU401</t>
+  </si>
+  <si>
+    <t>Ephemeral HPC to accelerate energy and utility workflows</t>
+  </si>
+  <si>
+    <t>Energy and utility companies use high performance computing (HPC) to design and optimize operations. Elastic, cloud-based HPC resources can dynamically provide the computational power needed for simulations on demand by creating reusable pipelines. HPC on AWS can be instantiated with the nodes and memory to optimize turnaround time while keeping the results sufficiently accurate. This allows you to make decisions about tradeoffs between cost, run time, and accuracy resolution based on your organization’s priorities. This chalk talk explores how to create HPC using infrastructure as code with AWS CloudFormation, Amazon EC2 Image Builder, Amazon FSx for Lustre, and inherited IAM permissions.</t>
+  </si>
+  <si>
+    <t>Abhishek Naik, Senior Solutions Architect</t>
+  </si>
+  <si>
+    <t>Kyle Jones, Sr. Manager</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Level 1, Room 104, MGM Grand</t>
+  </si>
+  <si>
+    <t>HPC, Energy</t>
+  </si>
+  <si>
+    <t>GEO032</t>
+  </si>
+  <si>
+    <t>Discover the full power of HPC on AWS and remove infrastructure constraints</t>
+  </si>
+  <si>
+    <t>This talk is delivered in Italian. High performance computing (HPC) has always been about utilizing the most effective technologies to solve the world’s most complex problems. However, many HPC users have been constrained by the need to purchase and deploy on-premises infrastructure to gain access to the best technologies for their applications. AWS HPC helps you innovate beyond the limitations of on-premises HPC infrastructure. In this talk, see how to create and manage HPC environments with AWS ParallelCluster, access 400 Gbps networking with Elastic Fabric Adapter, and chose from over 500 Amazon EC2 instances to run your largest, most complex HPC workloads in the cloud.</t>
+  </si>
+  <si>
+    <t>Geo Talk</t>
+  </si>
+  <si>
+    <t>Nicola Venuti, Principal Specialist Solution Architect</t>
+  </si>
+  <si>
+    <t>Level 1, Casanova Foyer- AWS Global Lounge, Venetian</t>
+  </si>
+  <si>
+    <t>PRT278</t>
+  </si>
+  <si>
+    <t>How Intel &amp; AWS collaborate to solve some of the world’s most urgent issues (sponsored by Intel)</t>
+  </si>
+  <si>
+    <t>AWS and Intel are committed to solving the world’s most critical social and environmental challenges through the power of HPC. Intel and AWS have collaborated to deliver first-rate engineering, resources, and results to impact customers around the world. Join this session to hear from Harvard Cancer Center, IKTOS, and Good Chemistry Co., who have utilized the scalability and availability of cloud computing powered by Intel to address problems spanning from cancer to ‘forever chemicals’ in water. This presentation is brought to you by Intel, an AWS Partner.</t>
+  </si>
+  <si>
+    <t>Tanner Marsh, Developer</t>
+  </si>
+  <si>
+    <t>HMS / VirtualFlow Project</t>
+  </si>
+  <si>
+    <t>Arman Zaribafiyan, CEO</t>
+  </si>
+  <si>
+    <t>Good Chemistry</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Upper Convention Promenade, Cristal 7, Wynn</t>
+  </si>
+  <si>
+    <t>HPC, Impact</t>
+  </si>
+  <si>
+    <t>CMP205-OF</t>
+  </si>
+  <si>
+    <t>Solve complex problems with pay-as-you-go infrastructure (Overflow room)</t>
+  </si>
+  <si>
+    <t>Level 1, Summit 231, Content Hub, Red Screen, Caesars Forum</t>
+  </si>
+  <si>
+    <t>PRT107</t>
+  </si>
+  <si>
+    <t>Faster drug discovery design with WEKA on AWS (sponsored by WEKA)</t>
+  </si>
+  <si>
+    <t>New methods like cryo-EM are enabling rapid advances in drug discovery. Using the right analysis workflow and tools are critical to success. In this lightning talk, join WEKA and Clovertex to learn how you can accelerate your drug design workflows using the WEKA data platform and Clovertex’s services on AWS. This presentation is brought to you by WEKA, an AWS Partner.</t>
+  </si>
+  <si>
+    <t>Lightning Talk</t>
+  </si>
+  <si>
+    <t>Baris Guler, Principal Architect</t>
+  </si>
+  <si>
+    <t>Hall B, Expo, Lightning Theater 2 , Booth #3543,</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>HPC, Storage</t>
+  </si>
+  <si>
+    <t>CMP220-OF</t>
+  </si>
+  <si>
+    <t>How AWS and aerospace and geospatial companies are rethinking HPC (Overflow room)</t>
+  </si>
+  <si>
+    <t>Level 2, Venetian E, Content Hub, Yellow Screen, Venetian</t>
+  </si>
+  <si>
+    <t>AWS Batch, Containers, Kubernetes</t>
+  </si>
+  <si>
+    <t>HPC, ParallelCluster, AWS Batch, EFA</t>
+  </si>
+  <si>
+    <t>HPC, ParallelCluster, AWS Batch, Geospatial, Open Data</t>
+  </si>
+  <si>
+    <t>HPC, EFA, ParallelCluster, AWS Batch</t>
+  </si>
+  <si>
+    <t>Eric Anderson, GM, Lustre / File Cache</t>
+  </si>
+  <si>
+    <t>Srinivas Tadepalli, Head of HPC GTM</t>
+  </si>
+  <si>
+    <t>Mark Galbraith, VP Productivity Engineering</t>
+  </si>
+  <si>
+    <t>Ana Simoes, Principal Specialist, ML Frameworks</t>
   </si>
 </sst>
 </file>
@@ -360,7 +618,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -383,6 +641,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Var(--font-family-base-ua1f64,&quot;"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF16191F"/>
+      <name val="Amazon Ember"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF16191F"/>
+      <name val="Var(--font-family-base-ua1f64,&quot;"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
+      <color rgb="FF16191F"/>
+      <name val="Amazon Ember"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -404,12 +685,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -724,36 +1016,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3922D00C-4E7C-1744-AE88-635DFF8D3D59}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="68.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.5" customWidth="1"/>
+    <col min="2" max="2" width="38.83203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="35.5" style="6" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" customWidth="1"/>
     <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16" customWidth="1"/>
-    <col min="15" max="15" width="54.5" customWidth="1"/>
-    <col min="16" max="16" width="30" customWidth="1"/>
+    <col min="9" max="9" width="18.5" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="11" max="11" width="7" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="56.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="43.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="17">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -777,7 +1072,7 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="11" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -796,111 +1091,117 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="289">
       <c r="A2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" t="s">
-        <v>57</v>
+        <v>103</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>105</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="E2">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="F2" t="s">
         <v>24</v>
       </c>
-      <c r="G2" t="s">
-        <v>79</v>
+      <c r="G2" s="7" t="s">
+        <v>189</v>
       </c>
       <c r="H2" t="s">
         <v>19</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J2" t="s">
+        <v>107</v>
       </c>
       <c r="K2" s="2">
         <v>44893</v>
       </c>
       <c r="L2" s="3">
-        <v>0.44791666666666669</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="M2" s="3">
-        <v>0.48958333333333331</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="N2" t="str">
-        <f t="shared" ref="N2:N16" si="0">TEXT(K2, "dddd")</f>
+        <f>TEXT(K2, "dddd")</f>
         <v>Monday</v>
       </c>
-      <c r="O2" s="4" t="s">
-        <v>93</v>
+      <c r="O2" s="8" t="s">
+        <v>108</v>
       </c>
       <c r="P2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" t="s">
-        <v>44</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="18">
+      <c r="A3" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>112</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E3">
         <v>300</v>
       </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" t="s">
-        <v>73</v>
+      <c r="F3">
+        <v>60</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>188</v>
       </c>
       <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" t="s">
-        <v>74</v>
+      <c r="I3" s="9" t="s">
+        <v>113</v>
       </c>
       <c r="J3" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="K3" s="2">
         <v>44893</v>
       </c>
       <c r="L3" s="3">
-        <v>0.66666666666666663</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="M3" s="3">
-        <v>0.70833333333333337</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="N3" t="str">
-        <f t="shared" si="0"/>
+        <f>TEXT(K3, "dddd")</f>
         <v>Monday</v>
       </c>
-      <c r="O3" s="4" t="s">
-        <v>89</v>
+      <c r="O3" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="P3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="18">
       <c r="A4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" t="s">
-        <v>37</v>
+        <v>116</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>118</v>
       </c>
       <c r="D4" t="s">
         <v>38</v>
@@ -908,269 +1209,297 @@
       <c r="E4">
         <v>300</v>
       </c>
-      <c r="F4" t="s">
-        <v>24</v>
+      <c r="F4">
+        <v>60</v>
       </c>
       <c r="G4" t="s">
-        <v>70</v>
+        <v>119</v>
       </c>
       <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>120</v>
+      </c>
+      <c r="J4" t="s">
         <v>19</v>
       </c>
       <c r="K4" s="2">
         <v>44893</v>
       </c>
       <c r="L4" s="3">
-        <v>0.72916666666666663</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="M4" s="3">
-        <v>0.77083333333333337</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="N4" t="str">
-        <f t="shared" si="0"/>
+        <f>TEXT(K4, "dddd")</f>
         <v>Monday</v>
       </c>
-      <c r="O4" s="4" t="s">
-        <v>87</v>
+      <c r="O4" s="8" t="s">
+        <v>121</v>
       </c>
       <c r="P4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="153">
       <c r="A5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" t="s">
-        <v>60</v>
+        <v>94</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="E5">
         <v>300</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H5" t="s">
         <v>19</v>
       </c>
       <c r="K5" s="2">
-        <v>44894</v>
+        <v>44893</v>
       </c>
       <c r="L5" s="3">
-        <v>0.58333333333333337</v>
+        <v>0.44791666666666669</v>
       </c>
       <c r="M5" s="3">
-        <v>0.66666666666666663</v>
+        <v>0.48958333333333331</v>
       </c>
       <c r="N5" t="str">
-        <f t="shared" si="0"/>
-        <v>Tuesday</v>
+        <f>TEXT(K5, "dddd")</f>
+        <v>Monday</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="P5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="340">
       <c r="A6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" t="s">
-        <v>41</v>
+        <v>123</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>125</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E6">
         <v>300</v>
       </c>
-      <c r="F6" t="s">
-        <v>24</v>
+      <c r="F6">
+        <v>60</v>
       </c>
       <c r="G6" t="s">
-        <v>71</v>
+        <v>190</v>
       </c>
       <c r="H6" t="s">
-        <v>19</v>
+        <v>126</v>
+      </c>
+      <c r="I6" t="s">
+        <v>127</v>
+      </c>
+      <c r="J6" t="s">
+        <v>128</v>
       </c>
       <c r="K6" s="2">
-        <v>44894</v>
+        <v>44893</v>
       </c>
       <c r="L6" s="3">
-        <v>0.67708333333333337</v>
+        <v>0.44791666666666669</v>
       </c>
       <c r="M6" s="3">
-        <v>0.71875</v>
-      </c>
-      <c r="N6" t="str">
-        <f t="shared" si="0"/>
-        <v>Tuesday</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>88</v>
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="N6" t="s">
+        <v>129</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>130</v>
       </c>
       <c r="P6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="289">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
+        <v>103</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>105</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="E7">
         <v>200</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" t="s">
-        <v>18</v>
+        <v>24</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>189</v>
       </c>
       <c r="H7" t="s">
         <v>19</v>
       </c>
+      <c r="I7" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="J7" t="s">
+        <v>107</v>
+      </c>
       <c r="K7" s="2">
-        <v>44894</v>
+        <v>44893</v>
       </c>
       <c r="L7" s="3">
-        <v>0.70833333333333337</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="M7" s="3">
-        <v>0.72222222222222221</v>
+        <v>0.61458333333333337</v>
       </c>
       <c r="N7" t="str">
-        <f t="shared" si="0"/>
-        <v>Tuesday</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>82</v>
+        <f>TEXT(K7, "dddd")</f>
+        <v>Monday</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>132</v>
       </c>
       <c r="P7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="272">
+      <c r="A8" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>135</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E8">
-        <v>300</v>
-      </c>
-      <c r="F8" t="s">
-        <v>61</v>
-      </c>
-      <c r="G8" t="s">
-        <v>69</v>
+        <v>400</v>
+      </c>
+      <c r="F8">
+        <v>60</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>136</v>
       </c>
       <c r="H8" t="s">
         <v>19</v>
       </c>
+      <c r="I8" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="J8" t="s">
+        <v>19</v>
+      </c>
       <c r="K8" s="2">
-        <v>44895</v>
+        <v>44893</v>
       </c>
       <c r="L8" s="3">
-        <v>0.38541666666666669</v>
+        <v>0.63541666666666663</v>
       </c>
       <c r="M8" s="3">
-        <v>0.46875</v>
-      </c>
-      <c r="N8" t="str">
-        <f t="shared" si="0"/>
-        <v>Wednesday</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>86</v>
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="N8" t="s">
+        <v>129</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="P8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="323">
       <c r="A9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" t="s">
-        <v>51</v>
+        <v>42</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="D9" t="s">
         <v>38</v>
       </c>
       <c r="E9">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="F9" t="s">
         <v>24</v>
       </c>
       <c r="G9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H9" t="s">
         <v>19</v>
       </c>
+      <c r="I9" t="s">
+        <v>74</v>
+      </c>
+      <c r="J9" t="s">
+        <v>75</v>
+      </c>
       <c r="K9" s="2">
-        <v>44895</v>
+        <v>44893</v>
       </c>
       <c r="L9" s="3">
-        <v>0.44791666666666669</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="M9" s="3">
-        <v>0.48958333333333331</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="N9" t="str">
-        <f t="shared" si="0"/>
-        <v>Wednesday</v>
+        <f>TEXT(K9, "dddd")</f>
+        <v>Monday</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="P9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="18">
       <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
+        <v>139</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>141</v>
       </c>
       <c r="D10" t="s">
         <v>23</v>
@@ -1178,50 +1507,43 @@
       <c r="E10">
         <v>200</v>
       </c>
-      <c r="F10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" t="s">
-        <v>62</v>
+      <c r="F10">
+        <v>60</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>142</v>
       </c>
       <c r="H10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" t="s">
-        <v>63</v>
-      </c>
-      <c r="J10" t="s">
-        <v>64</v>
+        <v>143</v>
       </c>
       <c r="K10" s="2">
-        <v>44895</v>
+        <v>44893</v>
       </c>
       <c r="L10" s="3">
-        <v>0.60416666666666663</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="M10" s="3">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="N10" t="str">
-        <f t="shared" si="0"/>
-        <v>Wednesday</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>83</v>
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="N10" t="s">
+        <v>129</v>
+      </c>
+      <c r="O10" s="9" t="s">
+        <v>144</v>
       </c>
       <c r="P10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="221">
       <c r="A11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" t="s">
-        <v>48</v>
+        <v>35</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="D11" t="s">
         <v>38</v>
@@ -1233,266 +1555,877 @@
         <v>24</v>
       </c>
       <c r="G11" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="H11" t="s">
         <v>19</v>
       </c>
       <c r="K11" s="2">
-        <v>44895</v>
+        <v>44893</v>
       </c>
       <c r="L11" s="3">
-        <v>0.69791666666666663</v>
+        <v>0.72916666666666663</v>
       </c>
       <c r="M11" s="3">
-        <v>0.73958333333333337</v>
+        <v>0.77083333333333337</v>
       </c>
       <c r="N11" t="str">
-        <f t="shared" si="0"/>
-        <v>Wednesday</v>
+        <f>TEXT(K11, "dddd")</f>
+        <v>Monday</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="P11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" t="s">
-        <v>30</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="34">
+      <c r="A12" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>148</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="E12">
-        <v>200</v>
-      </c>
-      <c r="F12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" t="s">
-        <v>68</v>
+        <v>400</v>
+      </c>
+      <c r="F12">
+        <v>60</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>149</v>
       </c>
       <c r="H12" t="s">
         <v>19</v>
       </c>
+      <c r="I12" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="J12" t="s">
+        <v>19</v>
+      </c>
       <c r="K12" s="2">
-        <v>44895</v>
+        <v>44894</v>
       </c>
       <c r="L12" s="3">
-        <v>0.79166666666666663</v>
+        <v>0.55208333333333337</v>
       </c>
       <c r="M12" s="3">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="N12" t="str">
-        <f t="shared" si="0"/>
-        <v>Wednesday</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>85</v>
+        <v>0.59375</v>
+      </c>
+      <c r="N12" t="s">
+        <v>151</v>
+      </c>
+      <c r="O12" s="8" t="s">
+        <v>152</v>
       </c>
       <c r="P12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="238">
       <c r="A13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" t="s">
-        <v>54</v>
+        <v>58</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="E13">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="F13" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="G13" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H13" t="s">
         <v>19</v>
       </c>
       <c r="K13" s="2">
-        <v>44895</v>
+        <v>44894</v>
       </c>
       <c r="L13" s="3">
-        <v>0.82291666666666663</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="M13" s="3">
-        <v>0.86458333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="N13" t="str">
-        <f t="shared" si="0"/>
-        <v>Wednesday</v>
+        <f>TEXT(K13, "dddd")</f>
+        <v>Tuesday</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="P13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>95</v>
-      </c>
-      <c r="B14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" t="s">
-        <v>57</v>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="34">
+      <c r="A14" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>156</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>157</v>
       </c>
       <c r="E14">
+        <v>100</v>
+      </c>
+      <c r="F14">
+        <v>60</v>
+      </c>
+      <c r="G14" t="s">
+        <v>158</v>
+      </c>
+      <c r="H14" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="2">
+        <v>44894</v>
+      </c>
+      <c r="L14" s="3">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="M14" s="3">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="N14" t="s">
+        <v>151</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="P14" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="323">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15">
         <v>300</v>
-      </c>
-      <c r="F14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G14" t="s">
-        <v>79</v>
-      </c>
-      <c r="H14" t="s">
-        <v>19</v>
-      </c>
-      <c r="K14" s="2">
-        <v>44896</v>
-      </c>
-      <c r="L14" s="3">
-        <v>0.61458333333333337</v>
-      </c>
-      <c r="M14" s="3">
-        <v>0.65625</v>
-      </c>
-      <c r="N14" t="str">
-        <f t="shared" si="0"/>
-        <v>Thursday</v>
-      </c>
-      <c r="O14" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="P14" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15">
-        <v>200</v>
       </c>
       <c r="F15" t="s">
         <v>24</v>
       </c>
       <c r="G15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="2">
+        <v>44894</v>
+      </c>
+      <c r="L15" s="3">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="M15" s="3">
+        <v>0.71875</v>
+      </c>
+      <c r="N15" t="str">
+        <f>TEXT(K15, "dddd")</f>
+        <v>Tuesday</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="P15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="204">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16">
+        <v>200</v>
+      </c>
+      <c r="F16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="2">
+        <v>44894</v>
+      </c>
+      <c r="L16" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="M16" s="3">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="N16" t="str">
+        <f>TEXT(K16, "dddd")</f>
+        <v>Tuesday</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="P16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="221">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17">
+        <v>300</v>
+      </c>
+      <c r="F17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="2">
+        <v>44895</v>
+      </c>
+      <c r="L17" s="3">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="M17" s="3">
+        <v>0.46875</v>
+      </c>
+      <c r="N17" t="str">
+        <f>TEXT(K17, "dddd")</f>
+        <v>Wednesday</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="P17" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="204">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18">
+        <v>400</v>
+      </c>
+      <c r="F18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" t="s">
+        <v>77</v>
+      </c>
+      <c r="H18" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="2">
+        <v>44895</v>
+      </c>
+      <c r="L18" s="3">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="M18" s="3">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="N18" t="str">
+        <f>TEXT(K18, "dddd")</f>
+        <v>Wednesday</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="P18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="18">
+      <c r="A19" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="D19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19">
+        <v>200</v>
+      </c>
+      <c r="F19">
+        <v>60</v>
+      </c>
+      <c r="G19" t="s">
+        <v>163</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="K19" s="2">
+        <v>44895</v>
+      </c>
+      <c r="L19" s="3">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="M19" s="3">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="N19" t="s">
+        <v>167</v>
+      </c>
+      <c r="O19" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="P19" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="323">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20">
+        <v>200</v>
+      </c>
+      <c r="F20" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20" t="s">
+        <v>63</v>
+      </c>
+      <c r="J20" t="s">
+        <v>64</v>
+      </c>
+      <c r="K20" s="2">
+        <v>44895</v>
+      </c>
+      <c r="L20" s="3">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="M20" s="3">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="N20" t="str">
+        <f>TEXT(K20, "dddd")</f>
+        <v>Wednesday</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="P20" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="323">
+      <c r="A21" t="s">
+        <v>170</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21">
+        <v>200</v>
+      </c>
+      <c r="F21">
+        <v>60</v>
+      </c>
+      <c r="G21" t="s">
+        <v>62</v>
+      </c>
+      <c r="H21" t="s">
+        <v>19</v>
+      </c>
+      <c r="I21" t="s">
+        <v>63</v>
+      </c>
+      <c r="J21" t="s">
+        <v>64</v>
+      </c>
+      <c r="K21" s="2">
+        <v>44895</v>
+      </c>
+      <c r="L21" s="3">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="M21" s="3">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="N21" t="str">
+        <f>TEXT(K21, "dddd")</f>
+        <v>Wednesday</v>
+      </c>
+      <c r="O21" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="P21" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="272">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22">
+        <v>300</v>
+      </c>
+      <c r="F22" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" t="s">
+        <v>76</v>
+      </c>
+      <c r="H22" t="s">
+        <v>19</v>
+      </c>
+      <c r="K22" s="2">
+        <v>44895</v>
+      </c>
+      <c r="L22" s="3">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="M22" s="3">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="N22" t="str">
+        <f>TEXT(K22, "dddd")</f>
+        <v>Wednesday</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="P22" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="340">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23">
+        <v>200</v>
+      </c>
+      <c r="F23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" t="s">
+        <v>68</v>
+      </c>
+      <c r="H23" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23" s="2">
+        <v>44895</v>
+      </c>
+      <c r="L23" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="M23" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="N23" t="str">
+        <f>TEXT(K23, "dddd")</f>
+        <v>Wednesday</v>
+      </c>
+      <c r="O23" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="P23" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="255">
+      <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24">
+        <v>400</v>
+      </c>
+      <c r="F24" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" t="s">
+        <v>78</v>
+      </c>
+      <c r="H24" t="s">
+        <v>19</v>
+      </c>
+      <c r="K24" s="2">
+        <v>44895</v>
+      </c>
+      <c r="L24" s="3">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="M24" s="3">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="N24" t="str">
+        <f>TEXT(K24, "dddd")</f>
+        <v>Wednesday</v>
+      </c>
+      <c r="O24" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="P24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="18">
+      <c r="A25" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="D25" t="s">
+        <v>176</v>
+      </c>
+      <c r="E25">
+        <v>100</v>
+      </c>
+      <c r="F25">
+        <v>60</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="H25" t="s">
+        <v>19</v>
+      </c>
+      <c r="K25" s="2">
+        <v>44896</v>
+      </c>
+      <c r="L25" s="3">
+        <v>0.52430555555555558</v>
+      </c>
+      <c r="M25" s="3">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="N25" t="s">
+        <v>179</v>
+      </c>
+      <c r="O25" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="P25" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="153">
+      <c r="A26" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26">
+        <v>300</v>
+      </c>
+      <c r="F26" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" t="s">
+        <v>79</v>
+      </c>
+      <c r="H26" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" s="2">
+        <v>44896</v>
+      </c>
+      <c r="L26" s="3">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="M26" s="3">
+        <v>0.65625</v>
+      </c>
+      <c r="N26" t="str">
+        <f>TEXT(K26, "dddd")</f>
+        <v>Thursday</v>
+      </c>
+      <c r="O26" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="P26" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="221">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27">
+        <v>200</v>
+      </c>
+      <c r="F27" t="s">
+        <v>24</v>
+      </c>
+      <c r="G27" t="s">
         <v>67</v>
       </c>
-      <c r="H15" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" t="s">
+      <c r="H27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I27" t="s">
         <v>65</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J27" t="s">
         <v>66</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K27" s="2">
         <v>44897</v>
       </c>
-      <c r="L15" s="3">
+      <c r="L27" s="3">
         <v>0.35416666666666669</v>
       </c>
-      <c r="M15" s="3">
+      <c r="M27" s="3">
         <v>0.39583333333333331</v>
       </c>
-      <c r="N15" t="str">
-        <f t="shared" si="0"/>
+      <c r="N27" t="str">
+        <f>TEXT(K27, "dddd")</f>
         <v>Friday</v>
       </c>
-      <c r="O15" s="4" t="s">
+      <c r="O27" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="P15" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="P27" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="221">
+      <c r="A28" t="s">
+        <v>181</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28">
+        <v>200</v>
+      </c>
+      <c r="F28" t="s">
+        <v>24</v>
+      </c>
+      <c r="G28" t="s">
+        <v>67</v>
+      </c>
+      <c r="H28" t="s">
+        <v>19</v>
+      </c>
+      <c r="I28" t="s">
+        <v>65</v>
+      </c>
+      <c r="J28" t="s">
+        <v>66</v>
+      </c>
+      <c r="K28" s="2">
+        <v>44897</v>
+      </c>
+      <c r="L28" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="M28" s="3">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="N28" t="str">
+        <f>TEXT(K28, "dddd")</f>
+        <v>Friday</v>
+      </c>
+      <c r="O28" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="P28" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="272">
+      <c r="A29" t="s">
         <v>46</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B29" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C29" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D29" t="s">
         <v>38</v>
       </c>
-      <c r="E16">
+      <c r="E29">
         <v>300</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F29" t="s">
         <v>24</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G29" t="s">
         <v>76</v>
       </c>
-      <c r="H16" t="s">
-        <v>19</v>
-      </c>
-      <c r="K16" s="2">
+      <c r="H29" t="s">
+        <v>19</v>
+      </c>
+      <c r="K29" s="2">
         <v>44897</v>
       </c>
-      <c r="L16" s="3">
+      <c r="L29" s="3">
         <v>0.41666666666666669</v>
       </c>
-      <c r="M16" s="3">
+      <c r="M29" s="3">
         <v>0.45833333333333331</v>
       </c>
-      <c r="N16" t="str">
-        <f t="shared" si="0"/>
+      <c r="N29" t="str">
+        <f>TEXT(K29, "dddd")</f>
         <v>Friday</v>
       </c>
-      <c r="O16" s="4" t="s">
+      <c r="O29" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="P16" t="s">
-        <v>98</v>
+      <c r="P29" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P16">
-    <sortCondition ref="K2:K16"/>
-    <sortCondition ref="L2:L16"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P29">
+    <sortCondition ref="K2:K29"/>
+    <sortCondition ref="L2:L29"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add CMP335-R1 to schedule
</commit_message>
<xml_diff>
--- a/scripts/reinvent-schedule.xlsx
+++ b/scripts/reinvent-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mwvaughn/src/websites/day1hpc.github.io/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50BFB3B-ADB0-2645-9246-59D5C982F777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70A4380-D99D-2C48-80A4-68326DEC8131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16640" xr2:uid="{D53CFD4F-014A-B641-809F-A5757838F61D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="194">
   <si>
     <t>Title</t>
   </si>
@@ -612,6 +612,9 @@
   </si>
   <si>
     <t>CMP211-R1</t>
+  </si>
+  <si>
+    <t>CMP335-R1</t>
   </si>
 </sst>
 </file>
@@ -1019,11 +1022,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3922D00C-4E7C-1744-AE88-635DFF8D3D59}">
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1094,7 +1097,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="289">
+    <row r="2" spans="1:16" ht="409.6">
       <c r="A2" t="s">
         <v>103</v>
       </c>
@@ -1247,7 +1250,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="153">
+    <row r="5" spans="1:16" ht="356">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -1292,7 +1295,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="340">
+    <row r="6" spans="1:16" ht="409.6">
       <c r="A6" t="s">
         <v>123</v>
       </c>
@@ -1342,7 +1345,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="289">
+    <row r="7" spans="1:16" ht="409.6">
       <c r="A7" t="s">
         <v>192</v>
       </c>
@@ -1393,7 +1396,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="272">
+    <row r="8" spans="1:16" ht="409.6">
       <c r="A8" s="9" t="s">
         <v>133</v>
       </c>
@@ -1443,7 +1446,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="323">
+    <row r="9" spans="1:16" ht="409.6">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1538,7 +1541,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="221">
+    <row r="11" spans="1:16" ht="409.6">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1633,7 +1636,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="238">
+    <row r="13" spans="1:16" ht="409.6">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -1678,7 +1681,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="34">
+    <row r="14" spans="1:16" ht="51">
       <c r="A14" s="9" t="s">
         <v>154</v>
       </c>
@@ -1722,7 +1725,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="323">
+    <row r="15" spans="1:16" ht="409.6">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -1767,7 +1770,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="204">
+    <row r="16" spans="1:16" ht="409.6">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1812,7 +1815,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="221">
+    <row r="17" spans="1:16" ht="409.6">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1857,7 +1860,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="204">
+    <row r="18" spans="1:16" ht="409.6">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -1902,65 +1905,60 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="18">
-      <c r="A19" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>162</v>
+    <row r="19" spans="1:16" ht="409.6">
+      <c r="A19" t="s">
+        <v>193</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="E19">
-        <v>200</v>
-      </c>
-      <c r="F19">
-        <v>60</v>
+        <v>300</v>
+      </c>
+      <c r="F19" t="s">
+        <v>61</v>
       </c>
       <c r="G19" t="s">
-        <v>163</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="J19" s="9" t="s">
-        <v>166</v>
+        <v>80</v>
+      </c>
+      <c r="H19" t="s">
+        <v>19</v>
       </c>
       <c r="K19" s="2">
         <v>44895</v>
       </c>
       <c r="L19" s="3">
-        <v>0.57291666666666663</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="M19" s="3">
-        <v>0.61458333333333337</v>
-      </c>
-      <c r="N19" t="s">
-        <v>167</v>
-      </c>
-      <c r="O19" s="9" t="s">
-        <v>168</v>
+        <v>0.5625</v>
+      </c>
+      <c r="N19" t="str">
+        <f>TEXT(K19, "dddd")</f>
+        <v>Wednesday</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>96</v>
       </c>
       <c r="P19" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="323">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>22</v>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="18">
+      <c r="A20" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>162</v>
       </c>
       <c r="D20" t="s">
         <v>23</v>
@@ -1968,47 +1966,46 @@
       <c r="E20">
         <v>200</v>
       </c>
-      <c r="F20" t="s">
-        <v>24</v>
+      <c r="F20">
+        <v>60</v>
       </c>
       <c r="G20" t="s">
-        <v>62</v>
-      </c>
-      <c r="H20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I20" t="s">
-        <v>63</v>
-      </c>
-      <c r="J20" t="s">
-        <v>64</v>
+        <v>163</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>166</v>
       </c>
       <c r="K20" s="2">
         <v>44895</v>
       </c>
       <c r="L20" s="3">
-        <v>0.60416666666666663</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="M20" s="3">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="N20" t="str">
-        <f>TEXT(K20, "dddd")</f>
-        <v>Wednesday</v>
-      </c>
-      <c r="O20" s="4" t="s">
-        <v>83</v>
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="N20" t="s">
+        <v>167</v>
+      </c>
+      <c r="O20" s="9" t="s">
+        <v>168</v>
       </c>
       <c r="P20" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="323">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="409.6">
       <c r="A21" t="s">
-        <v>170</v>
+        <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>171</v>
+        <v>21</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>22</v>
@@ -2019,8 +2016,8 @@
       <c r="E21">
         <v>200</v>
       </c>
-      <c r="F21">
-        <v>60</v>
+      <c r="F21" t="s">
+        <v>24</v>
       </c>
       <c r="G21" t="s">
         <v>62</v>
@@ -2047,79 +2044,85 @@
         <f>TEXT(K21, "dddd")</f>
         <v>Wednesday</v>
       </c>
-      <c r="O21" s="8" t="s">
-        <v>172</v>
+      <c r="O21" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="P21" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="272">
+    <row r="22" spans="1:16" ht="409.6">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>170</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>47</v>
+        <v>171</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="D22" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E22">
-        <v>300</v>
-      </c>
-      <c r="F22" t="s">
-        <v>24</v>
+        <v>200</v>
+      </c>
+      <c r="F22">
+        <v>60</v>
       </c>
       <c r="G22" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="H22" t="s">
         <v>19</v>
+      </c>
+      <c r="I22" t="s">
+        <v>63</v>
+      </c>
+      <c r="J22" t="s">
+        <v>64</v>
       </c>
       <c r="K22" s="2">
         <v>44895</v>
       </c>
       <c r="L22" s="3">
-        <v>0.69791666666666663</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="M22" s="3">
-        <v>0.73958333333333337</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="N22" t="str">
         <f>TEXT(K22, "dddd")</f>
         <v>Wednesday</v>
       </c>
-      <c r="O22" s="4" t="s">
-        <v>90</v>
+      <c r="O22" s="8" t="s">
+        <v>172</v>
       </c>
       <c r="P22" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="340">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="409.6">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="D23" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="E23">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="F23" t="s">
         <v>24</v>
       </c>
       <c r="G23" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="H23" t="s">
         <v>19</v>
@@ -2128,43 +2131,43 @@
         <v>44895</v>
       </c>
       <c r="L23" s="3">
-        <v>0.82291666666666663</v>
+        <v>0.69791666666666663</v>
       </c>
       <c r="M23" s="3">
-        <v>0.86458333333333337</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="N23" t="str">
         <f>TEXT(K23, "dddd")</f>
         <v>Wednesday</v>
       </c>
       <c r="O23" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="P23" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="255">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="409.6">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="E24">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F24" t="s">
         <v>24</v>
       </c>
       <c r="G24" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="H24" t="s">
         <v>19</v>
@@ -2183,77 +2186,78 @@
         <v>Wednesday</v>
       </c>
       <c r="O24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="P24" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="409.6">
+      <c r="A25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25">
+        <v>400</v>
+      </c>
+      <c r="F25" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25" t="s">
+        <v>78</v>
+      </c>
+      <c r="H25" t="s">
+        <v>19</v>
+      </c>
+      <c r="K25" s="2">
+        <v>44895</v>
+      </c>
+      <c r="L25" s="3">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="M25" s="3">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="N25" t="str">
+        <f>TEXT(K25, "dddd")</f>
+        <v>Wednesday</v>
+      </c>
+      <c r="O25" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="P24" t="s">
+      <c r="P25" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="18">
-      <c r="A25" s="9" t="s">
+    <row r="26" spans="1:16" ht="18">
+      <c r="A26" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B26" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C26" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>176</v>
       </c>
-      <c r="E25">
+      <c r="E26">
         <v>100</v>
       </c>
-      <c r="F25">
+      <c r="F26">
         <v>60</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="G26" s="9" t="s">
         <v>177</v>
-      </c>
-      <c r="H25" t="s">
-        <v>19</v>
-      </c>
-      <c r="K25" s="2">
-        <v>44896</v>
-      </c>
-      <c r="L25" s="3">
-        <v>0.52430555555555558</v>
-      </c>
-      <c r="M25" s="3">
-        <v>0.53472222222222221</v>
-      </c>
-      <c r="N25" t="s">
-        <v>179</v>
-      </c>
-      <c r="O25" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="P25" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="153">
-      <c r="A26" t="s">
-        <v>95</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" t="s">
-        <v>55</v>
-      </c>
-      <c r="E26">
-        <v>300</v>
-      </c>
-      <c r="F26" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26" t="s">
-        <v>79</v>
       </c>
       <c r="H26" t="s">
         <v>19</v>
@@ -2262,79 +2266,72 @@
         <v>44896</v>
       </c>
       <c r="L26" s="3">
-        <v>0.61458333333333337</v>
+        <v>0.52430555555555558</v>
       </c>
       <c r="M26" s="3">
-        <v>0.65625</v>
-      </c>
-      <c r="N26" t="str">
-        <f>TEXT(K26, "dddd")</f>
-        <v>Thursday</v>
-      </c>
-      <c r="O26" s="4" t="s">
-        <v>93</v>
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="N26" t="s">
+        <v>179</v>
+      </c>
+      <c r="O26" s="8" t="s">
+        <v>178</v>
       </c>
       <c r="P26" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="221">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="356">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="D27" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E27">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="F27" t="s">
         <v>24</v>
       </c>
       <c r="G27" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="H27" t="s">
         <v>19</v>
       </c>
-      <c r="I27" t="s">
-        <v>65</v>
-      </c>
-      <c r="J27" t="s">
-        <v>66</v>
-      </c>
       <c r="K27" s="2">
-        <v>44897</v>
+        <v>44896</v>
       </c>
       <c r="L27" s="3">
-        <v>0.35416666666666669</v>
+        <v>0.61458333333333337</v>
       </c>
       <c r="M27" s="3">
-        <v>0.39583333333333331</v>
+        <v>0.65625</v>
       </c>
       <c r="N27" t="str">
         <f>TEXT(K27, "dddd")</f>
-        <v>Friday</v>
+        <v>Thursday</v>
       </c>
       <c r="O27" s="4" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="P27" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="221">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="409.6">
       <c r="A28" t="s">
-        <v>181</v>
+        <v>25</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>182</v>
+        <v>26</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>27</v>
@@ -2373,62 +2370,113 @@
         <f>TEXT(K28, "dddd")</f>
         <v>Friday</v>
       </c>
-      <c r="O28" s="8" t="s">
-        <v>183</v>
+      <c r="O28" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="P28" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="272">
+    <row r="29" spans="1:16" ht="409.6">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>181</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>47</v>
+        <v>182</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E29">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="F29" t="s">
         <v>24</v>
       </c>
       <c r="G29" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="H29" t="s">
         <v>19</v>
+      </c>
+      <c r="I29" t="s">
+        <v>65</v>
+      </c>
+      <c r="J29" t="s">
+        <v>66</v>
       </c>
       <c r="K29" s="2">
         <v>44897</v>
       </c>
       <c r="L29" s="3">
-        <v>0.41666666666666669</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="M29" s="3">
-        <v>0.45833333333333331</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="N29" t="str">
         <f>TEXT(K29, "dddd")</f>
         <v>Friday</v>
       </c>
-      <c r="O29" s="4" t="s">
+      <c r="O29" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="P29" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="409.6">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30">
+        <v>300</v>
+      </c>
+      <c r="F30" t="s">
+        <v>24</v>
+      </c>
+      <c r="G30" t="s">
+        <v>76</v>
+      </c>
+      <c r="H30" t="s">
+        <v>19</v>
+      </c>
+      <c r="K30" s="2">
+        <v>44897</v>
+      </c>
+      <c r="L30" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="M30" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="N30" t="str">
+        <f>TEXT(K30, "dddd")</f>
+        <v>Friday</v>
+      </c>
+      <c r="O30" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="P29" t="s">
+      <c r="P30" t="s">
         <v>184</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P29">
-    <sortCondition ref="K2:K29"/>
-    <sortCondition ref="L2:L29"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P30">
+    <sortCondition ref="K2:K30"/>
+    <sortCondition ref="L2:L30"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>